<commit_message>
[Update] Add RTS and load with indexed address
</commit_message>
<xml_diff>
--- a/jeux d instructions.xlsx
+++ b/jeux d instructions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WS\sysnumapp\NanoProcessor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d428188c4adbc4b/Bureau/Project/NanoProcessor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120FADF4-9891-47BF-8C09-8CF8FD7FCC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{120FADF4-9891-47BF-8C09-8CF8FD7FCC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2FC7130-56AF-4E3F-991C-3ECCC7D28CF4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-3255" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,27 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$M$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$M$41</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="121">
   <si>
     <t xml:space="preserve">STOREaddr </t>
   </si>
@@ -345,19 +358,49 @@
     <t>CCR</t>
   </si>
   <si>
-    <t>MULU</t>
-  </si>
-  <si>
-    <t>accu * addr -&gt; accu2</t>
-  </si>
-  <si>
-    <t>Accu2_load</t>
-  </si>
-  <si>
     <t>TFR</t>
   </si>
   <si>
-    <t>msB de accu2 -&gt; accu</t>
+    <t>MULUaddr</t>
+  </si>
+  <si>
+    <t>MULUconst</t>
+  </si>
+  <si>
+    <t>LOADind</t>
+  </si>
+  <si>
+    <t>SecAccu_load</t>
+  </si>
+  <si>
+    <t>accu * const -&gt; accu &amp; secaccu</t>
+  </si>
+  <si>
+    <t>accu * DATA(addr)  -&gt; accu &amp; secaccu</t>
+  </si>
+  <si>
+    <t>secaccu -&gt; accu</t>
+  </si>
+  <si>
+    <t>LOADindconst</t>
+  </si>
+  <si>
+    <t>DATA(accu) -&gt; accu</t>
+  </si>
+  <si>
+    <t>LOADindaddr</t>
+  </si>
+  <si>
+    <t>DATA(accu+DATA(addr)) -&gt; accu</t>
+  </si>
+  <si>
+    <t>DATA(accu+const) -&gt; accu</t>
+  </si>
+  <si>
+    <t>RTS</t>
+  </si>
+  <si>
+    <t>accu -&gt; PC</t>
   </si>
 </sst>
 </file>
@@ -381,7 +424,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +446,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -504,22 +553,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -528,6 +561,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,7 +596,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -870,37 +919,38 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="1"/>
-    <col min="5" max="5" width="11.5546875" style="1"/>
-    <col min="6" max="7" width="11.44140625" style="1"/>
-    <col min="11" max="11" width="33.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1"/>
+    <col min="5" max="5" width="11.5703125" style="1"/>
+    <col min="6" max="7" width="11.42578125" style="1"/>
+    <col min="10" max="10" width="23.85546875" customWidth="1"/>
+    <col min="11" max="11" width="33.7109375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="25"/>
       <c r="G1" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="23"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I1" s="26"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>31</v>
       </c>
@@ -914,7 +964,7 @@
         <v>44</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>45</v>
@@ -935,7 +985,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -970,7 +1020,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
@@ -1005,7 +1055,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
@@ -1040,82 +1090,82 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="11" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="9" t="s">
+      <c r="C7" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H7" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I7" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>33</v>
@@ -1136,56 +1186,56 @@
         <v>40</v>
       </c>
       <c r="I8" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="17" t="s">
+      <c r="C9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I9" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>33</v>
@@ -1206,56 +1256,56 @@
         <v>40</v>
       </c>
       <c r="I10" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="9" t="s">
+      <c r="C11" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I11" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>82</v>
+        <v>6</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>33</v>
@@ -1270,62 +1320,62 @@
         <v>46</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H12" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="18" t="s">
-        <v>46</v>
+      <c r="I12" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="J12" s="18" t="s">
         <v>48</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>33</v>
@@ -1340,62 +1390,62 @@
         <v>46</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>40</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="J14" s="14" t="s">
         <v>48</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I15" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="J15" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I15" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>41</v>
+        <v>10</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>33</v>
@@ -1410,62 +1460,62 @@
         <v>46</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H16" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="J16" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K16" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" s="17" t="s">
+      <c r="C17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I17" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="J17" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K17" s="16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>46</v>
+        <v>12</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>33</v>
@@ -1480,479 +1530,479 @@
         <v>46</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="14" t="s">
-        <v>46</v>
+      <c r="I18" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="J18" s="14" t="s">
         <v>48</v>
       </c>
       <c r="K18" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K21" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="9" t="s">
+      <c r="C22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H22" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I19" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K19" s="11" t="s">
+      <c r="I22" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K22" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G20" s="9" t="s">
+      <c r="B23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H23" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="I20" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J20" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K20" s="11" t="s">
+      <c r="I23" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K23" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B24" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="17" t="s">
+      <c r="C24" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H24" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I21" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J21" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K21" s="16" t="s">
+      <c r="I24" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24" s="16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G22" s="17" t="s">
+      <c r="B25" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="H25" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="I22" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J22" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K22" s="16" t="s">
+      <c r="I25" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K25" s="16" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B26" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" s="9" t="s">
+      <c r="C26" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="H26" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J23" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K23" s="11" t="s">
+      <c r="I26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K26" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" s="9" t="s">
+      <c r="B27" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="H27" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="I24" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K24" s="11" t="s">
+      <c r="I27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K27" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="15" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" s="18" t="s">
+      <c r="B28" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="H25" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J25" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K25" s="16" t="s">
+      <c r="H28" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G26" s="18" t="s">
+      <c r="B29" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="H26" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I26" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J26" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K26" s="16" t="s">
+      <c r="H29" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J29" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K29" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G27" s="18" t="s">
+      <c r="B30" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="H27" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J27" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K27" s="16" t="s">
+      <c r="H30" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J30" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J28" s="14" t="s">
+      <c r="B31" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="K28" s="11" t="s">
+      <c r="K31" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H29" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I29" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J29" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="K29" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F30" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G30" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="H30" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I30" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J30" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="K30" s="16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G31" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="H31" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I31" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J31" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="K31" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
-        <v>25</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>42</v>
@@ -1982,47 +2032,47 @@
         <v>49</v>
       </c>
       <c r="K32" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J33" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J33" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="K33" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K33" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>42</v>
@@ -2052,182 +2102,345 @@
         <v>49</v>
       </c>
       <c r="K34" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G35" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J35" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I37" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J37" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="K37" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="15" t="s">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G35" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="H35" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I35" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J35" s="18" t="s">
+      <c r="B38" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I38" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J38" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="K35" s="16" t="s">
+      <c r="K38" s="16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H36" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I36" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K36" s="11" t="s">
+      <c r="B39" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H39" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J39" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K39" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="H37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J37" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K37" s="19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="24" t="s">
+      <c r="B41" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I41" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J41" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K41" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="G42" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H42" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J42" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="K42" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J43" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K43" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="B38" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="F38" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="G38" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="H38" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="I38" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="J38" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="K38" s="25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="D39" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="F39" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="G39" s="29" t="s">
+      <c r="B44" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G44" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="H39" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="I39" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="J39" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="K39" s="28" t="s">
-        <v>110</v>
+      <c r="H44" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="I44" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="J44" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="K44" s="22" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2251,16 +2464,16 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.44140625" style="1"/>
-    <col min="10" max="10" width="11.44140625" style="6"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.42578125" style="1"/>
+    <col min="10" max="10" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -2292,7 +2505,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2324,7 +2537,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2356,7 +2569,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2388,7 +2601,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2420,7 +2633,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2452,7 +2665,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2484,7 +2697,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2516,7 +2729,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2548,7 +2761,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2580,7 +2793,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2612,7 +2825,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2644,7 +2857,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2676,7 +2889,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2708,7 +2921,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2740,7 +2953,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2772,7 +2985,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2804,7 +3017,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2836,7 +3049,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2868,7 +3081,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>84</v>
       </c>
@@ -2900,7 +3113,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -2932,7 +3145,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -2964,7 +3177,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>86</v>
       </c>
@@ -2996,7 +3209,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -3028,7 +3241,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -3060,7 +3273,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -3092,7 +3305,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -3124,7 +3337,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -3156,7 +3369,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -3188,7 +3401,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -3220,7 +3433,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -3252,7 +3465,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -3284,7 +3497,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -3316,7 +3529,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -3348,7 +3561,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -3380,7 +3593,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -3423,7 +3636,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[Update] Add new opcode recently added in <Jeux d instructions.xlsx>
</commit_message>
<xml_diff>
--- a/jeux d instructions.xlsx
+++ b/jeux d instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d428188c4adbc4b/Bureau/Project/NanoProcessor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{120FADF4-9891-47BF-8C09-8CF8FD7FCC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2FC7130-56AF-4E3F-991C-3ECCC7D28CF4}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="13_ncr:1_{120FADF4-9891-47BF-8C09-8CF8FD7FCC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7BC2673-C91C-4701-8737-1AD10CEDCE20}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-3255" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$M$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$M$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="127">
   <si>
     <t xml:space="preserve">STOREaddr </t>
   </si>
@@ -358,18 +358,12 @@
     <t>CCR</t>
   </si>
   <si>
-    <t>TFR</t>
-  </si>
-  <si>
     <t>MULUaddr</t>
   </si>
   <si>
     <t>MULUconst</t>
   </si>
   <si>
-    <t>LOADind</t>
-  </si>
-  <si>
     <t>SecAccu_load</t>
   </si>
   <si>
@@ -385,22 +379,46 @@
     <t>LOADindconst</t>
   </si>
   <si>
-    <t>DATA(accu) -&gt; accu</t>
-  </si>
-  <si>
-    <t>LOADindaddr</t>
-  </si>
-  <si>
-    <t>DATA(accu+DATA(addr)) -&gt; accu</t>
-  </si>
-  <si>
     <t>DATA(accu+const) -&gt; accu</t>
   </si>
   <si>
     <t>RTS</t>
   </si>
   <si>
-    <t>accu -&gt; PC</t>
+    <t>TFRsecaccu</t>
+  </si>
+  <si>
+    <t>TFRaccu</t>
+  </si>
+  <si>
+    <t>INCsecaccu</t>
+  </si>
+  <si>
+    <t>DECsecaccu</t>
+  </si>
+  <si>
+    <t>secaccu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secaccu+ 1 -&gt; secaccu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">secaccu - 1 -&gt; secaccu </t>
+  </si>
+  <si>
+    <t>STOREsecaccu</t>
+  </si>
+  <si>
+    <t>accu -&gt; DATA(secaccu+const)</t>
+  </si>
+  <si>
+    <t>accu -&gt; secaccu</t>
+  </si>
+  <si>
+    <t>DATA(addr) -&gt; PC</t>
+  </si>
+  <si>
+    <t>DATA(addr+const)</t>
   </si>
 </sst>
 </file>
@@ -424,7 +442,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,12 +458,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -553,30 +565,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -593,6 +596,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -919,10 +926,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,22 +940,23 @@
     <col min="4" max="4" width="11.42578125" style="1"/>
     <col min="5" max="5" width="11.5703125" style="1"/>
     <col min="6" max="7" width="11.42578125" style="1"/>
-    <col min="10" max="10" width="23.85546875" customWidth="1"/>
-    <col min="11" max="11" width="33.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="40.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="26"/>
       <c r="G1" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="26"/>
+      <c r="I1" s="27"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -964,7 +972,7 @@
         <v>44</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>45</v>
@@ -986,116 +994,116 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="11" t="s">
+      <c r="B4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="16" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>93</v>
+      <c r="C5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>33</v>
@@ -1113,7 +1121,7 @@
         <v>35</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I6" s="18" t="s">
         <v>46</v>
@@ -1122,15 +1130,15 @@
         <v>48</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>115</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>114</v>
+        <v>2</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>33</v>
@@ -1148,24 +1156,24 @@
         <v>35</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>41</v>
+        <v>92</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="J7" s="18" t="s">
         <v>48</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>33</v>
@@ -1183,16 +1191,16 @@
         <v>35</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>40</v>
+        <v>126</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="J8" s="18" t="s">
         <v>48</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1791,46 +1799,46 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G26" s="9" t="s">
+      <c r="A26" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H26" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K26" s="11" t="s">
-        <v>102</v>
+      <c r="H26" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>42</v>
+        <v>85</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>82</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>33</v>
@@ -1848,91 +1856,91 @@
         <v>36</v>
       </c>
       <c r="H27" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="I27" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J27" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K27" s="11" t="s">
+      <c r="I28" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G28" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="H28" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J28" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K28" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="H29" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J29" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K29" s="16" t="s">
-        <v>70</v>
+      <c r="A29" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>46</v>
@@ -1962,485 +1970,567 @@
         <v>48</v>
       </c>
       <c r="K30" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J32" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K32" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J31" s="14" t="s">
+      <c r="B33" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J33" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="K31" s="11" t="s">
+      <c r="K33" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H32" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I32" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J32" s="14" t="s">
+      <c r="B34" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J34" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="K32" s="11" t="s">
+      <c r="K34" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G33" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="H33" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I33" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J33" s="18" t="s">
+      <c r="B35" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J35" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="K33" s="16" t="s">
+      <c r="K35" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G34" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="H34" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I34" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J34" s="18" t="s">
+      <c r="B36" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I36" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J36" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="K34" s="16" t="s">
+      <c r="K36" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H35" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I35" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J35" s="14" t="s">
+      <c r="B37" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J37" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="K35" s="11" t="s">
+      <c r="K37" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H36" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I36" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J36" s="14" t="s">
+      <c r="B38" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J38" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="K36" s="11" t="s">
+      <c r="K38" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="H37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I37" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J37" s="18" t="s">
+      <c r="B39" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I39" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J39" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="K37" s="16" t="s">
+      <c r="K39" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F38" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G38" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="H38" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I38" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J38" s="18" t="s">
+      <c r="B40" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I40" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J40" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="K38" s="16" t="s">
+      <c r="K40" s="16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H39" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I39" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K39" s="11" t="s">
+      <c r="B41" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J41" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K41" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J42" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="K42" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H43" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="B40" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="K40" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F41" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G41" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="H41" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I41" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J41" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K41" s="19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="B42" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="F42" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="G42" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="H42" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="I42" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J42" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="K42" s="30" t="s">
+      <c r="I43" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J43" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K43" s="19" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="J43" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K43" s="11" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H44" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I44" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J44" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K44" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B45" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G45" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H45" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J45" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="K45" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B44" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="F44" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G44" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="H44" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="I44" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="J44" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="K44" s="22" t="s">
-        <v>113</v>
+      <c r="B46" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K46" s="11" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Modify] Change view for print of instruction set architecture before to return
</commit_message>
<xml_diff>
--- a/jeux d instructions.xlsx
+++ b/jeux d instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d428188c4adbc4b/Bureau/Project/NanoProcessor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="187" documentId="13_ncr:1_{120FADF4-9891-47BF-8C09-8CF8FD7FCC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7BC2673-C91C-4701-8737-1AD10CEDCE20}"/>
+  <xr:revisionPtr revIDLastSave="188" documentId="13_ncr:1_{120FADF4-9891-47BF-8C09-8CF8FD7FCC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E98925D8-AD74-47EB-8200-2370F22AD42E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$M$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$M$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -596,10 +596,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -928,8 +924,8 @@
   </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="115" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,7 +2535,7 @@
     <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.84" bottom="0.33" header="0.41" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="74" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Tahoma,Gras"&amp;10Jeu d'instructions du nanoProcesseur</oddHeader>
   </headerFooter>

</xml_diff>